<commit_message>
When there is insufficient research in a genotype, the overall resistance level calculation is omitted and a footnote is displayed. Individual RASs are still given.
</commit_message>
<xml_diff>
--- a/tabular/contributed/SubtypeResistanceStrategy.xlsx
+++ b/tabular/contributed/SubtypeResistanceStrategy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13820" yWindow="3360" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="37300" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,80 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>(b) whether the drug is properly characterised in the literature for the genotype &amp; subtypes</t>
+  </si>
+  <si>
+    <t>Gt drug literature</t>
+  </si>
+  <si>
+    <t>Gt known</t>
+  </si>
+  <si>
+    <t>St known</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>St drug literature</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Match Gt</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Footnote / classification</t>
+  </si>
+  <si>
+    <t>Classification: Since the genotype is unknown, no resistance analysis was performed</t>
+  </si>
+  <si>
+    <t>Poor/None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This outlines which RASs should be included in the main analysis for a given drug and how they affect the report, based on </t>
+  </si>
+  <si>
+    <t>Match St or Gt-general</t>
+  </si>
+  <si>
+    <t>(a) the genotype (Gt) &amp; subtype (St) established for the sequence  -- if an unassigned subtype, this counts as "unknown".</t>
+  </si>
+  <si>
+    <t>RASs included</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Footnote: Since the subtype is unknown, resistant polymorphisms associated with other subtypes of genotype Y were included in the main analysis</t>
+  </si>
+  <si>
+    <t>Footnote: Since the resistance characteristics for drug X in subtype Y are not well understood, resistant polymorphisms associated other subtypes of genotype Z were included in the main analysis</t>
+  </si>
+  <si>
+    <t>Classification: "Since the resistance characteristics for drug X in genotype Y are not well understood, no resistance analysis was performed</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +410,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
for subtypes / drugs where research is insufficient, findings from other subtypes within the genotype are included in the main analysis.
</commit_message>
<xml_diff>
--- a/tabular/contributed/SubtypeResistanceStrategy.xlsx
+++ b/tabular/contributed/SubtypeResistanceStrategy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1440" windowWidth="37300" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="15620" yWindow="8420" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
resistance strategy doc update.
</commit_message>
<xml_diff>
--- a/tabular/contributed/SubtypeResistanceStrategy.xlsx
+++ b/tabular/contributed/SubtypeResistanceStrategy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15620" yWindow="8420" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="11200" yWindow="5620" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>